<commit_message>
Corrección guión, Esqueleto y solicitudes gráficas
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion11/EsqueletoGuion_CN_06_11_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion11/EsqueletoGuion_CN_06_11_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="18765" windowHeight="9195" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="18765" windowHeight="9195" tabRatio="729" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t>Los objetos que se encuentran en movimiento no lo hacen de la misma forma. Reconoce estos tipos de movimiento y las variables que intervienen</t>
   </si>
   <si>
-    <t>Bachillerato</t>
-  </si>
-  <si>
     <t>Ciencias Naturales</t>
   </si>
   <si>
@@ -266,6 +263,9 @@
   </si>
   <si>
     <t>CN_06_11_CO</t>
+  </si>
+  <si>
+    <t>Educación Básica Secundaria</t>
   </si>
 </sst>
 </file>
@@ -1581,7 +1581,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1591,8 +1591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1606,7 +1606,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1614,7 +1614,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1630,7 +1630,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1646,12 +1646,12 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1664,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1705,16 +1705,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="E2" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" s="14">
         <v>2</v>
@@ -1731,16 +1731,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="14">
         <v>3</v>
@@ -1751,16 +1751,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" s="14">
         <v>4</v>
@@ -1771,16 +1771,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" s="14">
         <v>5</v>
@@ -1791,16 +1791,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" s="14">
         <v>6</v>
@@ -1811,16 +1811,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7" s="15">
         <v>7</v>
@@ -1831,16 +1831,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" s="15">
         <v>8</v>
@@ -1851,16 +1851,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" s="15">
         <v>9</v>
@@ -1872,16 +1872,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F10" s="15">
         <v>10</v>
@@ -1893,16 +1893,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" s="15">
         <v>11</v>
@@ -1914,16 +1914,16 @@
         <v>6</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" s="15">
         <v>12</v>
@@ -1935,16 +1935,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F13" s="16">
         <v>13</v>
@@ -1955,16 +1955,16 @@
         <v>6</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F14" s="16">
         <v>14</v>
@@ -1975,16 +1975,16 @@
         <v>6</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F15" s="16">
         <v>15</v>
@@ -1995,16 +1995,16 @@
         <v>6</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16" s="16">
         <v>16</v>
@@ -2015,16 +2015,16 @@
         <v>6</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17" s="16">
         <v>17</v>
@@ -2035,16 +2035,16 @@
         <v>6</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F18" s="16">
         <v>18</v>
@@ -2055,16 +2055,16 @@
         <v>6</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F19" s="13">
         <v>19</v>
@@ -2075,16 +2075,16 @@
         <v>6</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F20" s="17">
         <v>20</v>
@@ -2095,16 +2095,16 @@
         <v>6</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F21" s="17">
         <v>21</v>
@@ -2115,16 +2115,16 @@
         <v>6</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F22" s="17">
         <v>22</v>
@@ -2135,16 +2135,16 @@
         <v>6</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="17" t="s">
         <v>77</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>78</v>
       </c>
       <c r="F23" s="17">
         <v>23</v>
@@ -2155,16 +2155,16 @@
         <v>6</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F24" s="17">
         <v>24</v>
@@ -2175,16 +2175,16 @@
         <v>6</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="33" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" s="33">
         <v>25</v>
@@ -2195,16 +2195,16 @@
         <v>6</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="33" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F26" s="33">
         <v>26</v>
@@ -2248,7 +2248,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1">
       <c r="A2" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>20</v>
@@ -2305,7 +2305,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -2316,7 +2316,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -2327,7 +2327,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -2338,7 +2338,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -2349,7 +2349,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -2360,7 +2360,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -2371,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -2382,7 +2382,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -2393,7 +2393,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -2404,7 +2404,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -2415,7 +2415,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -2426,7 +2426,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -2437,7 +2437,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -2448,7 +2448,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -2459,7 +2459,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -2470,7 +2470,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -2481,7 +2481,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
@@ -2492,7 +2492,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
@@ -2503,7 +2503,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
@@ -2514,7 +2514,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
@@ -2525,7 +2525,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
@@ -2536,7 +2536,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
@@ -2547,7 +2547,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
@@ -2558,7 +2558,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>19</v>
@@ -2653,10 +2653,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>23</v>
@@ -2670,10 +2670,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>24</v>
@@ -2687,10 +2687,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>26</v>
@@ -2704,10 +2704,10 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>25</v>
@@ -2717,7 +2717,7 @@
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>20</v>
@@ -2725,14 +2725,14 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>23</v>
@@ -2744,14 +2744,14 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>24</v>
@@ -2763,14 +2763,14 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>23</v>
@@ -2782,14 +2782,14 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>24</v>
@@ -2801,14 +2801,14 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>23</v>
@@ -2820,14 +2820,14 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>24</v>
@@ -2839,14 +2839,14 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>23</v>
@@ -2858,14 +2858,14 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>24</v>
@@ -2877,14 +2877,14 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>23</v>
@@ -2896,14 +2896,14 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>24</v>
@@ -2915,14 +2915,14 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>23</v>
@@ -2934,14 +2934,14 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>24</v>
@@ -2953,22 +2953,22 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="25" t="s">
         <v>56</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>57</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
       <c r="H18" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>19</v>
@@ -2976,14 +2976,14 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>30</v>
@@ -2995,14 +2995,14 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>25</v>
@@ -3010,7 +3010,7 @@
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
       <c r="H20" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>19</v>
@@ -3018,14 +3018,14 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>25</v>
@@ -3033,7 +3033,7 @@
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
       <c r="H21" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I21" s="14" t="s">
         <v>19</v>
@@ -3041,14 +3041,14 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>23</v>
@@ -3060,14 +3060,14 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>29</v>
@@ -3075,7 +3075,7 @@
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
       <c r="H23" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I23" s="14" t="s">
         <v>19</v>
@@ -3083,10 +3083,10 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>23</v>
@@ -3100,14 +3100,14 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E25" s="28" t="s">
         <v>23</v>
@@ -3119,14 +3119,14 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E26" s="28" t="s">
         <v>26</v>
@@ -3138,14 +3138,14 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E27" s="28" t="s">
         <v>23</v>
@@ -3157,14 +3157,14 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" s="28" t="s">
         <v>24</v>
@@ -3176,14 +3176,14 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" s="26"/>
       <c r="D29" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E29" s="28" t="s">
         <v>26</v>
@@ -3195,14 +3195,14 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E30" s="28" t="s">
         <v>23</v>
@@ -3214,18 +3214,18 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1">
       <c r="A31" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E31" s="28"/>
       <c r="F31" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G31" s="28" t="s">
         <v>23</v>
@@ -3235,18 +3235,18 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E32" s="28"/>
       <c r="F32" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G32" s="28" t="s">
         <v>24</v>
@@ -3256,18 +3256,18 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" s="26"/>
       <c r="D33" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E33" s="28"/>
       <c r="F33" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G33" s="28" t="s">
         <v>23</v>
@@ -3277,18 +3277,18 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" s="26"/>
       <c r="D34" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E34" s="28"/>
       <c r="F34" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G34" s="28" t="s">
         <v>24</v>
@@ -3298,18 +3298,18 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="26"/>
       <c r="D35" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E35" s="28"/>
       <c r="F35" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G35" s="28" t="s">
         <v>30</v>
@@ -3319,18 +3319,18 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C36" s="26"/>
       <c r="D36" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E36" s="28"/>
       <c r="F36" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G36" s="28" t="s">
         <v>23</v>
@@ -3340,18 +3340,18 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" s="26"/>
       <c r="D37" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E37" s="28"/>
       <c r="F37" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G37" s="28" t="s">
         <v>26</v>
@@ -3361,24 +3361,24 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" s="26"/>
       <c r="D38" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E38" s="28"/>
       <c r="F38" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G38" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I38" s="15" t="s">
         <v>19</v>
@@ -3386,18 +3386,18 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" s="26"/>
       <c r="D39" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E39" s="28"/>
       <c r="F39" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G39" s="28" t="s">
         <v>23</v>
@@ -3407,24 +3407,24 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C40" s="26"/>
       <c r="D40" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E40" s="28"/>
       <c r="F40" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G40" s="28" t="s">
         <v>25</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I40" s="15" t="s">
         <v>19</v>
@@ -3432,24 +3432,24 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41" s="26"/>
       <c r="D41" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E41" s="28"/>
       <c r="F41" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G41" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I41" s="15" t="s">
         <v>19</v>
@@ -3457,18 +3457,18 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C42" s="26"/>
       <c r="D42" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E42" s="28"/>
       <c r="F42" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G42" s="28" t="s">
         <v>23</v>
@@ -3478,14 +3478,14 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E43" s="28" t="s">
         <v>23</v>
@@ -3497,14 +3497,14 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E44" s="28" t="s">
         <v>26</v>
@@ -3516,14 +3516,14 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45" s="26"/>
       <c r="D45" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E45" s="28" t="s">
         <v>23</v>
@@ -3535,14 +3535,14 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C46" s="26"/>
       <c r="D46" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E46" s="28" t="s">
         <v>29</v>
@@ -3550,7 +3550,7 @@
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
       <c r="H46" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I46" s="15" t="s">
         <v>19</v>
@@ -3558,14 +3558,14 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C47" s="26"/>
       <c r="D47" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E47" s="28" t="s">
         <v>25</v>
@@ -3573,7 +3573,7 @@
       <c r="F47" s="28"/>
       <c r="G47" s="28"/>
       <c r="H47" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I47" s="15" t="s">
         <v>19</v>
@@ -3581,14 +3581,14 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C48" s="26"/>
       <c r="D48" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E48" s="28" t="s">
         <v>23</v>
@@ -3600,14 +3600,14 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" s="26"/>
       <c r="D49" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E49" s="28" t="s">
         <v>29</v>
@@ -3615,7 +3615,7 @@
       <c r="F49" s="28"/>
       <c r="G49" s="28"/>
       <c r="H49" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I49" s="15" t="s">
         <v>19</v>
@@ -3623,14 +3623,14 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" s="26"/>
       <c r="D50" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>29</v>
@@ -3638,7 +3638,7 @@
       <c r="F50" s="28"/>
       <c r="G50" s="28"/>
       <c r="H50" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I50" s="15" t="s">
         <v>19</v>
@@ -3646,10 +3646,10 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>23</v>
@@ -3663,14 +3663,14 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52" s="16"/>
       <c r="D52" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>23</v>
@@ -3682,14 +3682,14 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>26</v>
@@ -3701,14 +3701,14 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>23</v>
@@ -3720,14 +3720,14 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" s="16"/>
       <c r="D55" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>26</v>
@@ -3739,14 +3739,14 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56" s="16"/>
       <c r="D56" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E56" s="16" t="s">
         <v>30</v>
@@ -3758,14 +3758,14 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57" s="16"/>
       <c r="D57" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E57" s="16" t="s">
         <v>29</v>
@@ -3773,7 +3773,7 @@
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
       <c r="H57" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I57" s="16" t="s">
         <v>19</v>
@@ -3781,14 +3781,14 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" s="16"/>
       <c r="D58" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>23</v>
@@ -3800,14 +3800,14 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59" s="16"/>
       <c r="D59" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>30</v>
@@ -3819,14 +3819,14 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C60" s="16"/>
       <c r="D60" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>26</v>
@@ -3838,14 +3838,14 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C61" s="16"/>
       <c r="D61" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>23</v>
@@ -3857,14 +3857,14 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C62" s="16"/>
       <c r="D62" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E62" s="16" t="s">
         <v>26</v>
@@ -3876,18 +3876,18 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C63" s="16"/>
       <c r="D63" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E63" s="16"/>
       <c r="F63" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G63" s="16" t="s">
         <v>23</v>
@@ -3897,18 +3897,18 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C64" s="16"/>
       <c r="D64" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E64" s="16"/>
       <c r="F64" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G64" s="16" t="s">
         <v>26</v>
@@ -3918,18 +3918,18 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C65" s="16"/>
       <c r="D65" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E65" s="16"/>
       <c r="F65" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G65" s="16" t="s">
         <v>24</v>
@@ -3939,18 +3939,18 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E66" s="16"/>
       <c r="F66" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G66" s="16" t="s">
         <v>23</v>
@@ -3960,18 +3960,18 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C67" s="24"/>
       <c r="D67" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E67" s="24"/>
       <c r="F67" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G67" s="30" t="s">
         <v>24</v>
@@ -3981,24 +3981,24 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C68" s="16"/>
       <c r="D68" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E68" s="16"/>
       <c r="F68" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G68" s="16" t="s">
         <v>25</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I68" s="16" t="s">
         <v>19</v>
@@ -4006,24 +4006,24 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E69" s="16"/>
       <c r="F69" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G69" s="16" t="s">
         <v>29</v>
       </c>
       <c r="H69" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I69" s="16" t="s">
         <v>19</v>
@@ -4031,18 +4031,18 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C70" s="16"/>
       <c r="D70" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E70" s="16"/>
       <c r="F70" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G70" s="16" t="s">
         <v>23</v>
@@ -4052,18 +4052,18 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C71" s="16"/>
       <c r="D71" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E71" s="16"/>
       <c r="F71" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G71" s="16" t="s">
         <v>26</v>
@@ -4073,18 +4073,18 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C72" s="16"/>
       <c r="D72" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E72" s="16"/>
       <c r="F72" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G72" s="16" t="s">
         <v>23</v>
@@ -4094,18 +4094,18 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C73" s="16"/>
       <c r="D73" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E73" s="16"/>
       <c r="F73" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G73" s="16" t="s">
         <v>24</v>
@@ -4115,18 +4115,18 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C74" s="16"/>
       <c r="D74" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E74" s="16"/>
       <c r="F74" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G74" s="16" t="s">
         <v>23</v>
@@ -4136,24 +4136,24 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C75" s="16"/>
       <c r="D75" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E75" s="16"/>
       <c r="F75" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G75" s="16" t="s">
         <v>25</v>
       </c>
       <c r="H75" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I75" s="16" t="s">
         <v>19</v>
@@ -4161,24 +4161,24 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C76" s="16"/>
       <c r="D76" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E76" s="16"/>
       <c r="F76" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G76" s="16" t="s">
         <v>29</v>
       </c>
       <c r="H76" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I76" s="16" t="s">
         <v>19</v>
@@ -4186,14 +4186,14 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C77" s="16"/>
       <c r="D77" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E77" s="16" t="s">
         <v>23</v>
@@ -4205,14 +4205,14 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C78" s="16"/>
       <c r="D78" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E78" s="16" t="s">
         <v>29</v>
@@ -4220,7 +4220,7 @@
       <c r="F78" s="16"/>
       <c r="G78" s="16"/>
       <c r="H78" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I78" s="16" t="s">
         <v>19</v>
@@ -4228,10 +4228,10 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C79" s="23" t="s">
         <v>23</v>
@@ -4245,14 +4245,14 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C80" s="23"/>
       <c r="D80" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E80" s="23" t="s">
         <v>23</v>
@@ -4264,14 +4264,14 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C81" s="23"/>
       <c r="D81" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E81" s="23" t="s">
         <v>24</v>
@@ -4283,14 +4283,14 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C82" s="23"/>
       <c r="D82" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E82" s="23" t="s">
         <v>23</v>
@@ -4302,14 +4302,14 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C83" s="23"/>
       <c r="D83" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E83" s="23" t="s">
         <v>24</v>
@@ -4321,14 +4321,14 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C84" s="23"/>
       <c r="D84" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E84" s="23" t="s">
         <v>25</v>
@@ -4336,7 +4336,7 @@
       <c r="F84" s="23"/>
       <c r="G84" s="23"/>
       <c r="H84" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I84" s="23" t="s">
         <v>19</v>
@@ -4344,14 +4344,14 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C85" s="23"/>
       <c r="D85" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E85" s="23" t="s">
         <v>23</v>
@@ -4363,14 +4363,14 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C86" s="23"/>
       <c r="D86" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E86" s="23" t="s">
         <v>24</v>
@@ -4382,14 +4382,14 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C87" s="23"/>
       <c r="D87" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E87" s="23" t="s">
         <v>23</v>
@@ -4401,10 +4401,10 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B88" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C88" s="31" t="s">
         <v>23</v>
@@ -4418,10 +4418,10 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B89" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C89" s="31" t="s">
         <v>29</v>
@@ -4431,7 +4431,7 @@
       <c r="F89" s="31"/>
       <c r="G89" s="31"/>
       <c r="H89" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I89" s="31" t="s">
         <v>19</v>
@@ -4439,10 +4439,10 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B90" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C90" s="31" t="s">
         <v>29</v>
@@ -4452,7 +4452,7 @@
       <c r="F90" s="31"/>
       <c r="G90" s="31"/>
       <c r="H90" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I90" s="31" t="s">
         <v>19</v>
@@ -4460,10 +4460,10 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B91" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C91" s="31" t="s">
         <v>29</v>
@@ -4473,7 +4473,7 @@
       <c r="F91" s="31"/>
       <c r="G91" s="31"/>
       <c r="H91" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I91" s="31" t="s">
         <v>19</v>
@@ -4481,10 +4481,10 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B92" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C92" s="31" t="s">
         <v>29</v>
@@ -4494,7 +4494,7 @@
       <c r="F92" s="31"/>
       <c r="G92" s="31"/>
       <c r="H92" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I92" s="31" t="s">
         <v>19</v>
@@ -4502,10 +4502,10 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B93" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C93" s="31" t="s">
         <v>29</v>
@@ -4515,7 +4515,7 @@
       <c r="F93" s="31"/>
       <c r="G93" s="31"/>
       <c r="H93" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I93" s="31" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Última revisión, modificación de esqueleto
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion11/EsqueletoGuion_CN_06_11_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion11/EsqueletoGuion_CN_06_11_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="18765" windowHeight="9195" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="18765" windowHeight="9195" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="84">
   <si>
     <t>FICHA</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Recuerda</t>
   </si>
   <si>
-    <t>Los objetos que se encuentran en movimiento no lo hacen de la misma forma. Reconoce estos tipos de movimiento y las variables que intervienen</t>
-  </si>
-  <si>
     <t>Ciencias Naturales</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>CN</t>
   </si>
   <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: El movimiento </t>
-  </si>
-  <si>
     <t>Introducción al movimiento</t>
   </si>
   <si>
@@ -145,42 +139,12 @@
     <t>Refuerza tu aprendizaje: Concepto de movimiento</t>
   </si>
   <si>
-    <t>Definición de velocidad</t>
-  </si>
-  <si>
-    <t>Unidades para medir la velocidad</t>
-  </si>
-  <si>
-    <t>Relaciona las unidades</t>
-  </si>
-  <si>
     <t>Realiza cálculos con la aceleración</t>
   </si>
   <si>
-    <t>Definición de aceleración</t>
-  </si>
-  <si>
     <t>La velocidad</t>
   </si>
   <si>
-    <t>Definiciones de los elementos del movimiento</t>
-  </si>
-  <si>
-    <t>Practica el movimiento uniforme</t>
-  </si>
-  <si>
-    <t>Realiza observaciones sobre la gráfica distancia-tiempo</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje:  La gráfica velocidad contra tiempo</t>
-  </si>
-  <si>
-    <t>Realiza los cálculos sobre velocidad.- tiempo</t>
-  </si>
-  <si>
-    <t>El Rozamiento</t>
-  </si>
-  <si>
     <t>Competencias: estudio sobre el movimiento de los cuerpos</t>
   </si>
   <si>
@@ -190,9 +154,6 @@
     <t>Competencias: comprensión de la actuación de la gravedad</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje:  Movimiento  y sistema de referencia</t>
-  </si>
-  <si>
     <t>Trayectoria y desplazamiento</t>
   </si>
   <si>
@@ -238,30 +199,15 @@
     <t>Competencias</t>
   </si>
   <si>
-    <t>Relaciona las Unidades</t>
-  </si>
-  <si>
-    <t>Interpreta la gráfica</t>
-  </si>
-  <si>
-    <t>Construye una gráfica velocidad contra tiempo</t>
-  </si>
-  <si>
     <t>La Fuerza de rozamiento</t>
   </si>
   <si>
-    <t>El rozamiento</t>
-  </si>
-  <si>
     <t>Competencias: cálculo de la velocidad de un móvil</t>
   </si>
   <si>
     <t>Competencias: análisis de los diferentes tipos de movimiento</t>
   </si>
   <si>
-    <t>CN_06_11</t>
-  </si>
-  <si>
     <t>CN_06_11_CO</t>
   </si>
   <si>
@@ -269,6 +215,69 @@
   </si>
   <si>
     <t>Mapa Conceptual</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>El movimiento y la velocidad</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: El movimiento</t>
+  </si>
+  <si>
+    <t>MN_3C_23</t>
+  </si>
+  <si>
+    <t>2° ESO</t>
+  </si>
+  <si>
+    <t>CN_08_10</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Las características del movimiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conoce la velocidad de cualquier movimiento </t>
+  </si>
+  <si>
+    <t>Las unidades para medir la velocidad</t>
+  </si>
+  <si>
+    <t>Relaciona las unidades de velocidad más comunes</t>
+  </si>
+  <si>
+    <t>Entiende qué es la aceleración</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La velocidad</t>
+  </si>
+  <si>
+    <t>Conoce las definiciones de movimiento</t>
+  </si>
+  <si>
+    <t>Practica el movimiento rectilíneo uniforme</t>
+  </si>
+  <si>
+    <t>La gráfica de movimiento distancia-tiempo</t>
+  </si>
+  <si>
+    <t>Realiza cálculos sobre distancia-tiempo</t>
+  </si>
+  <si>
+    <t>Cómo se construye una gráfica velocidad-tiempo</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La gráfica velocidad-tiempo</t>
+  </si>
+  <si>
+    <t>Realiza cálculos sobre velocidad-tiempo</t>
+  </si>
+  <si>
+    <t>Movimiento  y sistema de referencia</t>
+  </si>
+  <si>
+    <t>Los objetos que se encuentran en movimiento no lo hacen de la misma forma. Reconoce estos tipos de movimiento y las variables que intervienen.</t>
   </si>
 </sst>
 </file>
@@ -1607,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,7 +1631,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1630,7 +1639,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1638,7 +1647,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1646,7 +1655,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1662,7 +1671,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1681,7 +1690,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="D20" sqref="D20:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,16 +1730,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F2" s="14">
         <v>2</v>
@@ -1743,82 +1752,82 @@
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
-        <v>6</v>
+      <c r="A3" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="E3" s="14" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F3" s="14">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
-        <v>6</v>
+      <c r="A4" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F4" s="14">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
-        <v>6</v>
+      <c r="A5" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F5" s="14">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="A6" s="15">
         <v>6</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="14">
+      <c r="B6" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="15">
         <v>6</v>
       </c>
     </row>
@@ -1827,16 +1836,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F7" s="15">
         <v>7</v>
@@ -1847,36 +1856,36 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F8" s="15">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
-        <v>6</v>
+      <c r="A9" s="15" t="s">
+        <v>67</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F9" s="15">
         <v>9</v>
@@ -1888,16 +1897,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F10" s="15">
         <v>10</v>
@@ -1909,16 +1918,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F11" s="15">
         <v>11</v>
@@ -1926,20 +1935,20 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
-        <v>6</v>
+      <c r="A12" s="15" t="s">
+        <v>67</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F12" s="15">
         <v>12</v>
@@ -1947,60 +1956,60 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
-        <v>6</v>
+      <c r="A13" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F13" s="16">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
-        <v>6</v>
+      <c r="A14" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F14" s="16">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
-        <v>6</v>
+      <c r="A15" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F15" s="16">
         <v>15</v>
@@ -2011,16 +2020,16 @@
         <v>6</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F16" s="16">
         <v>16</v>
@@ -2031,36 +2040,36 @@
         <v>6</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F17" s="16">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
-        <v>6</v>
+      <c r="A18" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F18" s="16">
         <v>18</v>
@@ -2071,16 +2080,16 @@
         <v>6</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F19" s="13">
         <v>19</v>
@@ -2091,16 +2100,16 @@
         <v>6</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F20" s="17">
         <v>20</v>
@@ -2111,16 +2120,16 @@
         <v>6</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F21" s="17">
         <v>21</v>
@@ -2131,16 +2140,16 @@
         <v>6</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F22" s="17">
         <v>22</v>
@@ -2151,16 +2160,16 @@
         <v>6</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F23" s="17">
         <v>23</v>
@@ -2171,16 +2180,16 @@
         <v>6</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F24" s="17">
         <v>24</v>
@@ -2202,7 +2211,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2224,7 +2233,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>20</v>
@@ -2235,7 +2244,7 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>20</v>
@@ -2274,8 +2283,8 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2301,7 +2310,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -2312,7 +2321,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -2323,7 +2332,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -2334,7 +2343,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -2345,7 +2354,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -2356,7 +2365,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -2367,7 +2376,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -2378,7 +2387,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -2389,7 +2398,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -2400,7 +2409,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -2411,7 +2420,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -2422,7 +2431,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -2433,7 +2442,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -2444,7 +2453,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -2455,7 +2464,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -2466,7 +2475,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -2477,7 +2486,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
@@ -2488,7 +2497,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
@@ -2499,7 +2508,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
@@ -2510,7 +2519,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
@@ -2521,7 +2530,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
@@ -2532,7 +2541,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
@@ -2543,7 +2552,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
@@ -2554,7 +2563,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
         <v>19</v>
@@ -2601,8 +2610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+    <sheetView topLeftCell="E1" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2649,10 +2658,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>23</v>
@@ -2666,10 +2675,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>24</v>
@@ -2683,10 +2692,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>26</v>
@@ -2700,10 +2709,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>25</v>
@@ -2713,7 +2722,7 @@
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="14" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>20</v>
@@ -2721,14 +2730,14 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>23</v>
@@ -2740,14 +2749,14 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>24</v>
@@ -2759,14 +2768,14 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>23</v>
@@ -2778,14 +2787,14 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>24</v>
@@ -2797,14 +2806,14 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>23</v>
@@ -2816,14 +2825,14 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>24</v>
@@ -2835,14 +2844,14 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>23</v>
@@ -2854,14 +2863,14 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>24</v>
@@ -2873,14 +2882,14 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>23</v>
@@ -2892,14 +2901,14 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E15" s="25" t="s">
         <v>24</v>
@@ -2911,14 +2920,14 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E16" s="25" t="s">
         <v>23</v>
@@ -2930,14 +2939,14 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>24</v>
@@ -2949,22 +2958,22 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
       <c r="H18" s="14" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>19</v>
@@ -2972,14 +2981,14 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>30</v>
@@ -2991,14 +3000,14 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>25</v>
@@ -3006,7 +3015,7 @@
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
       <c r="H20" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>19</v>
@@ -3014,14 +3023,14 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="19" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>25</v>
@@ -3029,7 +3038,7 @@
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
       <c r="H21" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I21" s="14" t="s">
         <v>19</v>
@@ -3037,14 +3046,14 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="19" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>23</v>
@@ -3056,14 +3065,14 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="19" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>29</v>
@@ -3071,7 +3080,7 @@
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
       <c r="H23" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I23" s="14" t="s">
         <v>19</v>
@@ -3079,10 +3088,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>23</v>
@@ -3096,14 +3105,14 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E25" s="28" t="s">
         <v>23</v>
@@ -3115,14 +3124,14 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E26" s="28" t="s">
         <v>26</v>
@@ -3134,14 +3143,14 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E27" s="28" t="s">
         <v>23</v>
@@ -3153,14 +3162,14 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E28" s="28" t="s">
         <v>24</v>
@@ -3172,14 +3181,14 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C29" s="26"/>
       <c r="D29" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E29" s="28" t="s">
         <v>26</v>
@@ -3191,14 +3200,14 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E30" s="28" t="s">
         <v>23</v>
@@ -3210,18 +3219,18 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E31" s="28"/>
       <c r="F31" s="28" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G31" s="28" t="s">
         <v>23</v>
@@ -3231,18 +3240,18 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E32" s="28"/>
       <c r="F32" s="28" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G32" s="28" t="s">
         <v>24</v>
@@ -3252,18 +3261,18 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C33" s="26"/>
       <c r="D33" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E33" s="28"/>
       <c r="F33" s="28" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G33" s="28" t="s">
         <v>23</v>
@@ -3273,18 +3282,18 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C34" s="26"/>
       <c r="D34" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E34" s="28"/>
       <c r="F34" s="28" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G34" s="28" t="s">
         <v>24</v>
@@ -3294,18 +3303,18 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C35" s="26"/>
       <c r="D35" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E35" s="28"/>
       <c r="F35" s="28" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G35" s="28" t="s">
         <v>30</v>
@@ -3315,18 +3324,18 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C36" s="26"/>
       <c r="D36" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E36" s="28"/>
       <c r="F36" s="28" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G36" s="28" t="s">
         <v>23</v>
@@ -3336,18 +3345,18 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C37" s="26"/>
       <c r="D37" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E37" s="28"/>
       <c r="F37" s="28" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G37" s="28" t="s">
         <v>26</v>
@@ -3357,24 +3366,24 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C38" s="26"/>
       <c r="D38" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E38" s="28"/>
       <c r="F38" s="28" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G38" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="I38" s="15" t="s">
         <v>19</v>
@@ -3382,18 +3391,18 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C39" s="26"/>
       <c r="D39" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E39" s="28"/>
       <c r="F39" s="28" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G39" s="28" t="s">
         <v>23</v>
@@ -3403,24 +3412,24 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C40" s="26"/>
       <c r="D40" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E40" s="28"/>
       <c r="F40" s="28" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G40" s="28" t="s">
         <v>25</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="I40" s="15" t="s">
         <v>19</v>
@@ -3428,24 +3437,24 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C41" s="26"/>
       <c r="D41" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E41" s="28"/>
       <c r="F41" s="28" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G41" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I41" s="15" t="s">
         <v>19</v>
@@ -3453,18 +3462,18 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C42" s="26"/>
       <c r="D42" s="27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E42" s="28"/>
       <c r="F42" s="28" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G42" s="28" t="s">
         <v>23</v>
@@ -3474,14 +3483,14 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="27" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E43" s="28" t="s">
         <v>23</v>
@@ -3493,14 +3502,14 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="27" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E44" s="28" t="s">
         <v>26</v>
@@ -3512,14 +3521,14 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C45" s="26"/>
       <c r="D45" s="27" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E45" s="28" t="s">
         <v>23</v>
@@ -3531,14 +3540,14 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C46" s="26"/>
       <c r="D46" s="27" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E46" s="28" t="s">
         <v>29</v>
@@ -3546,7 +3555,7 @@
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
       <c r="H46" s="15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I46" s="15" t="s">
         <v>19</v>
@@ -3554,14 +3563,14 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C47" s="26"/>
       <c r="D47" s="27" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E47" s="28" t="s">
         <v>25</v>
@@ -3569,7 +3578,7 @@
       <c r="F47" s="28"/>
       <c r="G47" s="28"/>
       <c r="H47" s="15" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="I47" s="15" t="s">
         <v>19</v>
@@ -3577,14 +3586,14 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C48" s="26"/>
       <c r="D48" s="27" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E48" s="28" t="s">
         <v>23</v>
@@ -3596,14 +3605,14 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C49" s="26"/>
       <c r="D49" s="27" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E49" s="28" t="s">
         <v>29</v>
@@ -3611,7 +3620,7 @@
       <c r="F49" s="28"/>
       <c r="G49" s="28"/>
       <c r="H49" s="15" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="I49" s="15" t="s">
         <v>19</v>
@@ -3619,14 +3628,14 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C50" s="26"/>
       <c r="D50" s="27" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>29</v>
@@ -3634,7 +3643,7 @@
       <c r="F50" s="28"/>
       <c r="G50" s="28"/>
       <c r="H50" s="15" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="I50" s="15" t="s">
         <v>19</v>
@@ -3642,10 +3651,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>23</v>
@@ -3659,14 +3668,14 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C52" s="16"/>
       <c r="D52" s="16" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>23</v>
@@ -3678,14 +3687,14 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>26</v>
@@ -3697,14 +3706,14 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>23</v>
@@ -3716,14 +3725,14 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C55" s="16"/>
       <c r="D55" s="16" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>26</v>
@@ -3735,14 +3744,14 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C56" s="16"/>
       <c r="D56" s="16" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E56" s="16" t="s">
         <v>30</v>
@@ -3754,14 +3763,14 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C57" s="16"/>
       <c r="D57" s="16" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E57" s="16" t="s">
         <v>29</v>
@@ -3769,7 +3778,7 @@
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
       <c r="H57" s="16" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="I57" s="16" t="s">
         <v>19</v>
@@ -3777,14 +3786,14 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C58" s="16"/>
       <c r="D58" s="16" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>23</v>
@@ -3796,14 +3805,14 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C59" s="16"/>
       <c r="D59" s="16" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>30</v>
@@ -3815,14 +3824,14 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C60" s="16"/>
       <c r="D60" s="16" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>26</v>
@@ -3834,14 +3843,14 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C61" s="16"/>
       <c r="D61" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>23</v>
@@ -3853,14 +3862,14 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C62" s="16"/>
       <c r="D62" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E62" s="16" t="s">
         <v>26</v>
@@ -3872,18 +3881,18 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C63" s="16"/>
       <c r="D63" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E63" s="16"/>
       <c r="F63" s="16" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G63" s="16" t="s">
         <v>23</v>
@@ -3893,18 +3902,18 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C64" s="16"/>
       <c r="D64" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E64" s="16"/>
       <c r="F64" s="16" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G64" s="16" t="s">
         <v>26</v>
@@ -3914,18 +3923,18 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C65" s="16"/>
       <c r="D65" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E65" s="16"/>
       <c r="F65" s="16" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G65" s="16" t="s">
         <v>24</v>
@@ -3935,18 +3944,18 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E66" s="16"/>
       <c r="F66" s="16" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G66" s="16" t="s">
         <v>23</v>
@@ -3956,18 +3965,18 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C67" s="24"/>
       <c r="D67" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E67" s="24"/>
       <c r="F67" s="16" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G67" s="30" t="s">
         <v>24</v>
@@ -3977,24 +3986,24 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C68" s="16"/>
       <c r="D68" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E68" s="16"/>
       <c r="F68" s="16" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G68" s="16" t="s">
         <v>25</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="I68" s="16" t="s">
         <v>19</v>
@@ -4002,24 +4011,24 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E69" s="16"/>
       <c r="F69" s="16" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G69" s="16" t="s">
         <v>29</v>
       </c>
       <c r="H69" s="16" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="I69" s="16" t="s">
         <v>19</v>
@@ -4027,18 +4036,18 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C70" s="16"/>
       <c r="D70" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E70" s="16"/>
       <c r="F70" s="16" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G70" s="16" t="s">
         <v>23</v>
@@ -4048,18 +4057,18 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C71" s="16"/>
       <c r="D71" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E71" s="16"/>
       <c r="F71" s="16" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G71" s="16" t="s">
         <v>26</v>
@@ -4069,18 +4078,18 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C72" s="16"/>
       <c r="D72" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E72" s="16"/>
       <c r="F72" s="16" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G72" s="16" t="s">
         <v>23</v>
@@ -4090,18 +4099,18 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C73" s="16"/>
       <c r="D73" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E73" s="16"/>
       <c r="F73" s="16" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G73" s="16" t="s">
         <v>24</v>
@@ -4111,18 +4120,18 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C74" s="16"/>
       <c r="D74" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E74" s="16"/>
       <c r="F74" s="16" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G74" s="16" t="s">
         <v>23</v>
@@ -4132,24 +4141,24 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C75" s="16"/>
       <c r="D75" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E75" s="16"/>
       <c r="F75" s="16" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G75" s="16" t="s">
         <v>25</v>
       </c>
       <c r="H75" s="16" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="I75" s="16" t="s">
         <v>19</v>
@@ -4157,24 +4166,24 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C76" s="16"/>
       <c r="D76" s="16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E76" s="16"/>
       <c r="F76" s="16" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G76" s="16" t="s">
         <v>29</v>
       </c>
       <c r="H76" s="16" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="I76" s="16" t="s">
         <v>19</v>
@@ -4182,14 +4191,14 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C77" s="16"/>
       <c r="D77" s="16" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E77" s="16" t="s">
         <v>23</v>
@@ -4201,14 +4210,14 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C78" s="16"/>
       <c r="D78" s="16" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E78" s="16" t="s">
         <v>29</v>
@@ -4216,7 +4225,7 @@
       <c r="F78" s="16"/>
       <c r="G78" s="16"/>
       <c r="H78" s="16" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="I78" s="16" t="s">
         <v>19</v>
@@ -4224,10 +4233,10 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C79" s="23" t="s">
         <v>23</v>
@@ -4241,14 +4250,14 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C80" s="23"/>
       <c r="D80" s="23" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E80" s="23" t="s">
         <v>23</v>
@@ -4260,14 +4269,14 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C81" s="23"/>
       <c r="D81" s="23" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E81" s="23" t="s">
         <v>24</v>
@@ -4279,14 +4288,14 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C82" s="23"/>
       <c r="D82" s="23" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E82" s="23" t="s">
         <v>23</v>
@@ -4298,14 +4307,14 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C83" s="23"/>
       <c r="D83" s="23" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E83" s="23" t="s">
         <v>24</v>
@@ -4317,22 +4326,22 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C84" s="23"/>
       <c r="D84" s="23" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E84" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F84" s="23"/>
       <c r="G84" s="23"/>
-      <c r="H84" s="23" t="s">
-        <v>74</v>
+      <c r="H84" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="I84" s="23" t="s">
         <v>19</v>
@@ -4340,14 +4349,14 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C85" s="23"/>
       <c r="D85" s="23" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E85" s="23" t="s">
         <v>23</v>
@@ -4359,14 +4368,14 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C86" s="23"/>
       <c r="D86" s="23" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E86" s="23" t="s">
         <v>24</v>
@@ -4378,14 +4387,14 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C87" s="23"/>
       <c r="D87" s="23" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E87" s="23" t="s">
         <v>23</v>
@@ -4397,10 +4406,10 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B88" s="31" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C88" s="31" t="s">
         <v>23</v>
@@ -4414,10 +4423,10 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B89" s="31" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C89" s="31" t="s">
         <v>29</v>
@@ -4426,8 +4435,8 @@
       <c r="E89" s="31"/>
       <c r="F89" s="31"/>
       <c r="G89" s="31"/>
-      <c r="H89" s="31" t="s">
-        <v>51</v>
+      <c r="H89" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="I89" s="31" t="s">
         <v>19</v>
@@ -4435,10 +4444,10 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B90" s="31" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C90" s="31" t="s">
         <v>29</v>
@@ -4447,8 +4456,8 @@
       <c r="E90" s="31"/>
       <c r="F90" s="31"/>
       <c r="G90" s="31"/>
-      <c r="H90" s="31" t="s">
-        <v>52</v>
+      <c r="H90" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="I90" s="31" t="s">
         <v>19</v>
@@ -4456,10 +4465,10 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B91" s="31" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C91" s="31" t="s">
         <v>29</v>
@@ -4468,8 +4477,8 @@
       <c r="E91" s="31"/>
       <c r="F91" s="31"/>
       <c r="G91" s="31"/>
-      <c r="H91" s="31" t="s">
-        <v>75</v>
+      <c r="H91" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="I91" s="31" t="s">
         <v>19</v>
@@ -4477,10 +4486,10 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B92" s="31" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C92" s="31" t="s">
         <v>29</v>
@@ -4489,8 +4498,8 @@
       <c r="E92" s="31"/>
       <c r="F92" s="31"/>
       <c r="G92" s="31"/>
-      <c r="H92" s="31" t="s">
-        <v>76</v>
+      <c r="H92" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="I92" s="31" t="s">
         <v>19</v>
@@ -4498,10 +4507,10 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B93" s="31" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C93" s="31" t="s">
         <v>29</v>
@@ -4510,8 +4519,8 @@
       <c r="E93" s="31"/>
       <c r="F93" s="31"/>
       <c r="G93" s="31"/>
-      <c r="H93" s="31" t="s">
-        <v>53</v>
+      <c r="H93" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="I93" s="31" t="s">
         <v>19</v>

</xml_diff>